<commit_message>
Updated following manuscript revision
Updated following manuscript revision
</commit_message>
<xml_diff>
--- a/meta/ld_mapping.xlsx
+++ b/meta/ld_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abbieschindler/Documents/Schindler_Lab/Data/RFID_VDM/meta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abbieschindler/Documents/Schindler_Lab/Manuscripts/2022/2022_RFIDVDM/github/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B9B63C-03C2-FE42-BB51-B54228662C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8529E9AF-1B79-774C-8621-CAFF69784840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36200" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{45B94316-19C3-1B46-BFE2-314A60E884C8}"/>
+    <workbookView xWindow="-38220" yWindow="960" windowWidth="13080" windowHeight="16260" xr2:uid="{45B94316-19C3-1B46-BFE2-314A60E884C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="68">
   <si>
     <t>light</t>
   </si>
@@ -596,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625B1098-CE81-2C47-8F55-F87B6236A371}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,7 +643,7 @@
         <v>67</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>67</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>67</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>67</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -741,7 +741,7 @@
         <v>67</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
         <v>67</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>67</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>67</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -825,7 +825,7 @@
         <v>67</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -853,7 +853,7 @@
         <v>67</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -867,7 +867,7 @@
         <v>67</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -895,7 +895,7 @@
         <v>67</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -909,7 +909,7 @@
         <v>67</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>67</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -951,7 +951,7 @@
         <v>67</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -993,7 +993,7 @@
         <v>67</v>
       </c>
       <c r="D28">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1008,412 +1008,6 @@
       </c>
       <c r="D29">
         <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>13</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>14</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>15</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>15</v>
-      </c>
-      <c r="B44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>15</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>16</v>
-      </c>
-      <c r="B46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>16</v>
-      </c>
-      <c r="B47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>16</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>17</v>
-      </c>
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>17</v>
-      </c>
-      <c r="B50" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>17</v>
-      </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>18</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>18</v>
-      </c>
-      <c r="B53" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>18</v>
-      </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>19</v>
-      </c>
-      <c r="B55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>19</v>
-      </c>
-      <c r="B56" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>19</v>
-      </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>20</v>
-      </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>